<commit_message>
Some edits in the 4SF form descriptions
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-4SF-update.xlsx
+++ b/form_reporting_templates/Form-4SF-update.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\Dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B9D692-C154-4720-8F65-B0C58766E40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DDC38E-C4AF-4475-B1EC-DCE9CF577CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="jbPe6SBLf4oG4Cgxdp2GTHPCnTakxOLusQvs3FLR97ZGw7ZrHwFP80gs+fK1zVtwmXmlsYM45w/LTktaEDAlHA==" workbookSaltValue="+e6btQraNKSRCi9yKssXHA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Liaison officer</t>
+  </si>
+  <si>
+    <t>Size class(high)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,16 +255,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -810,13 +803,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,10 +831,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -905,6 +887,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1248,24 +1241,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="60"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1315,15 +1308,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="60"/>
+      <c r="G8" s="57"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1366,7 +1359,7 @@
       <c r="C12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="59"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1377,7 +1370,7 @@
       <c r="C13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="59"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1492,10 +1485,10 @@
       <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="60"/>
+      <c r="G24" s="57"/>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1627,11 +1620,11 @@
     </row>
     <row r="36" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="69"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="66"/>
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1684,7 +1677,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C098252-FABC-4161-882E-794F98E79BC6}">
-  <dimension ref="B1:H55"/>
+  <dimension ref="B1:I55"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -1699,537 +1692,595 @@
     <col min="2" max="2" width="11.42578125" style="38" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="39" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="40" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="52" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="42" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="43" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="42" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
-      <c r="G1" s="41"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="41"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="61" t="s">
+      <c r="I1" s="41"/>
+    </row>
+    <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-    </row>
-    <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="70" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="53" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="45" t="s">
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="69"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="I5" s="47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
       <c r="C6" s="24"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="53"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="54"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="54"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="27"/>
       <c r="D9" s="28"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="54"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="31"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
       <c r="D10" s="28"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="31"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="54"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
       <c r="C11" s="27"/>
       <c r="D11" s="28"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="31"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="54"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="26"/>
       <c r="C12" s="27"/>
       <c r="D12" s="28"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="54"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="C13" s="27"/>
       <c r="D13" s="28"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="54"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="26"/>
       <c r="C14" s="27"/>
       <c r="D14" s="28"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="54"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="54"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="26"/>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="54"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="26"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="54"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="26"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="54"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="54"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="54"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="26"/>
       <c r="C21" s="27"/>
       <c r="D21" s="28"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="54"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
       <c r="D22" s="28"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="54"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="26"/>
       <c r="C23" s="27"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="31"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E23" s="54"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="26"/>
       <c r="C24" s="27"/>
       <c r="D24" s="28"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="31"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="54"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="26"/>
       <c r="C25" s="27"/>
       <c r="D25" s="28"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="31"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="54"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="31"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="26"/>
       <c r="C26" s="27"/>
       <c r="D26" s="28"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="31"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="54"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="31"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="26"/>
       <c r="C27" s="27"/>
       <c r="D27" s="28"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="31"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="54"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="26"/>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="31"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="54"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="31"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
       <c r="D29" s="28"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="54"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="31"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="26"/>
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="31"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E30" s="54"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="31"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="26"/>
       <c r="C31" s="27"/>
       <c r="D31" s="28"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="31"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="54"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="26"/>
       <c r="C32" s="27"/>
       <c r="D32" s="28"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="31"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E32" s="54"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="31"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="26"/>
       <c r="C33" s="27"/>
       <c r="D33" s="28"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="31"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="54"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="31"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="26"/>
       <c r="C34" s="27"/>
       <c r="D34" s="28"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="31"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E34" s="54"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="31"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="26"/>
       <c r="C35" s="27"/>
       <c r="D35" s="28"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="31"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E35" s="54"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="31"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="26"/>
       <c r="C36" s="27"/>
       <c r="D36" s="28"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="31"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E36" s="54"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="31"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="31"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="54"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="31"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="26"/>
       <c r="C38" s="27"/>
       <c r="D38" s="28"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="31"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E38" s="54"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="31"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="26"/>
       <c r="C39" s="27"/>
       <c r="D39" s="28"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="31"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="54"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="31"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="26"/>
       <c r="C40" s="27"/>
       <c r="D40" s="28"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="31"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E40" s="54"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="31"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="26"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="31"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E41" s="54"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="31"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="26"/>
       <c r="C42" s="27"/>
       <c r="D42" s="28"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="31"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E42" s="54"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="31"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="26"/>
       <c r="C43" s="27"/>
       <c r="D43" s="28"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="31"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E43" s="54"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="26"/>
       <c r="C44" s="27"/>
       <c r="D44" s="28"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="31"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E44" s="54"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="31"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="26"/>
       <c r="C45" s="27"/>
       <c r="D45" s="28"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="31"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E45" s="54"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="31"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="26"/>
       <c r="C46" s="27"/>
       <c r="D46" s="28"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="31"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E46" s="54"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="31"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="26"/>
       <c r="C47" s="27"/>
       <c r="D47" s="28"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="31"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E47" s="54"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="26"/>
       <c r="C48" s="27"/>
       <c r="D48" s="28"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="31"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="54"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="26"/>
       <c r="C49" s="27"/>
       <c r="D49" s="28"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="31"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E49" s="54"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="31"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="26"/>
       <c r="C50" s="27"/>
       <c r="D50" s="28"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="31"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E50" s="54"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="31"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="26"/>
       <c r="C51" s="27"/>
       <c r="D51" s="28"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="31"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E51" s="54"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="31"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="26"/>
       <c r="C52" s="27"/>
       <c r="D52" s="28"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="31"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E52" s="54"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="31"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="26"/>
       <c r="C53" s="27"/>
       <c r="D53" s="28"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="31"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E53" s="54"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="31"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="26"/>
       <c r="C54" s="27"/>
       <c r="D54" s="28"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="31"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E54" s="54"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="31"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="26"/>
       <c r="C55" s="27"/>
       <c r="D55" s="28"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="31"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="31"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wmVtbRueG3kaf//pcdenUYVGWnSDwgfyyRAThZiJJQYjOGaztl/Ze1cZ0mZSBpSeJm38foea4IReCmvPHU3Z6g==" saltValue="P6y6U3V/jwdg5DjSSRaQKA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nIg5TyvbedcJpP+3TA62WB0QVv3mXUWbWbBRQ9rGqEgLUUOFikJuefHVapxLybkzo2b0D/B2Yy/g0p30Hmxj+w==" saltValue="e/j9xG2GXh6s+fSUtcneGA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="3">
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="F4:I4"/>
     <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:H1048576">
+  <conditionalFormatting sqref="B6:I1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>B6=""</formula>
     </cfRule>

</xml_diff>